<commit_message>
Validação no import de excel
</commit_message>
<xml_diff>
--- a/clientes_para_importar.xlsx
+++ b/clientes_para_importar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gkolndor\desenv\Projetos\desafiobeca\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82E4619-C1B2-403D-8708-6EB6A0FB10CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7DF94FA-4883-430C-AEEE-BEBD809288E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FA699844-AA00-4EE8-9121-ECA0CDAE8B89}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{FA699844-AA00-4EE8-9121-ECA0CDAE8B89}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="158">
   <si>
     <t>Nome</t>
   </si>
@@ -507,6 +507,9 @@
   </si>
   <si>
     <t>558.326.080-70</t>
+  </si>
+  <si>
+    <t>703.124.040-93</t>
   </si>
 </sst>
 </file>
@@ -601,7 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -625,6 +628,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -965,7 +971,7 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1555,7 +1561,7 @@
       <c r="A13" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="9" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -1606,7 +1612,7 @@
         <v>121</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="D14" s="4">
         <v>30862</v>
@@ -1709,7 +1715,10 @@
       <c r="O16" s="7"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B13" r:id="rId1" xr:uid="{0950DDF6-16AB-4DA7-916C-100EFF5E8163}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>